<commit_message>
updated figs, notebooks, data
</commit_message>
<xml_diff>
--- a/data/table.xlsx
+++ b/data/table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>GNU_guix</t>
   </si>
@@ -25,6 +25,9 @@
     <t>bioconda</t>
   </si>
   <si>
+    <t>bioconductor</t>
+  </si>
+  <si>
     <t>biolinux</t>
   </si>
   <si>
@@ -53,9 +56,6 @@
   </si>
   <si>
     <t>Var1</t>
-  </si>
-  <si>
-    <t>bioconductor</t>
   </si>
 </sst>
 </file>
@@ -413,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -459,8 +459,11 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,8 +503,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -515,34 +521,37 @@
         <v>225</v>
       </c>
       <c r="E3">
+        <v>23</v>
+      </c>
+      <c r="F3">
         <v>198</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>398</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>236</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>404</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1640</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2106</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>444</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
       <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -556,36 +565,39 @@
         <v>6385</v>
       </c>
       <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4">
         <v>61</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>97</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>64</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>318</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>79</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>750</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>387</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
       <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -597,36 +609,39 @@
         <v>14</v>
       </c>
       <c r="E5">
+        <v>1823</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>12</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>17</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>14</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>196</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>6</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
       <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -638,36 +653,39 @@
         <v>61</v>
       </c>
       <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
         <v>308</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
       </c>
       <c r="G6">
         <v>7</v>
       </c>
       <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
         <v>57</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>14</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>42</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>51</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -679,36 +697,39 @@
         <v>97</v>
       </c>
       <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>5960</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>137</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>445</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>453</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>3196</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>796</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
       <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -720,36 +741,39 @@
         <v>64</v>
       </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>137</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>14918</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>100</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>160</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2040</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>86</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
       <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -761,36 +785,39 @@
         <v>318</v>
       </c>
       <c r="E9">
+        <v>17</v>
+      </c>
+      <c r="F9">
         <v>57</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>445</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>100</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1836</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>423</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>692</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>627</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
       <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -805,33 +832,36 @@
         <v>14</v>
       </c>
       <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
         <v>453</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>160</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>423</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>4828</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1175</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>521</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
       <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -843,36 +873,39 @@
         <v>750</v>
       </c>
       <c r="E11">
+        <v>196</v>
+      </c>
+      <c r="F11">
         <v>42</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>3196</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2040</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>692</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1175</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>184655</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>438</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>1</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>347</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -884,36 +917,39 @@
         <v>387</v>
       </c>
       <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
         <v>51</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>796</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>86</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>627</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>521</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>438</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>3451</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
       <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -940,21 +976,24 @@
         <v>0</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>1</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
       <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>9370</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -966,30 +1005,33 @@
         <v>17</v>
       </c>
       <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>171</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>42</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>172</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>244</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>347</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>161</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
       <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <v>1692</v>
       </c>
     </row>

</xml_diff>